<commit_message>
Analyzed the way to store images for a photo.
</commit_message>
<xml_diff>
--- a/设计/HTTP接口.xlsx
+++ b/设计/HTTP接口.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\HummingBird\设计\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23324\Documents\Codes\Hummingbird\设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2665F5C0-31BF-4734-A4F7-47D5EEDCAD08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAD7CCB-F126-4A8E-BA3A-D98CD4DA2788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="17550" yWindow="10095" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="资源列表" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
   <si>
     <t>资源</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -178,10 +178,6 @@
   </si>
   <si>
     <t>√</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>×</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -526,10 +522,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>/api/post</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>POST</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -654,6 +646,10 @@
   </si>
   <si>
     <t>数字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/post</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1346,7 +1342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1461,9 +1457,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1492,9 +1485,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
@@ -1517,6 +1507,24 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1552,24 +1560,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1860,23 +1850,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="9.75" customWidth="1"/>
-    <col min="6" max="6" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="22.58203125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="17" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="11.375" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="28" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1896,25 +1886,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="81" t="s">
+    <row r="2" spans="1:15" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:15" ht="20.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="83"/>
-      <c r="J4" s="74" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
+      <c r="J4" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="76"/>
-    </row>
-    <row r="5" spans="1:15" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="80"/>
+    </row>
+    <row r="5" spans="1:15" ht="28" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1946,12 +1936,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>11</v>
@@ -1978,7 +1968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="29" t="s">
         <v>8</v>
       </c>
@@ -1991,7 +1981,7 @@
       <c r="E7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="88" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="33" t="s">
@@ -2010,7 +2000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" s="29" t="s">
         <v>20</v>
       </c>
@@ -2023,7 +2013,7 @@
       <c r="E8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="85"/>
+      <c r="F8" s="89"/>
       <c r="J8" s="33" t="s">
         <v>16</v>
       </c>
@@ -2040,7 +2030,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
@@ -2054,25 +2044,25 @@
         <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="M9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="56" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
@@ -2086,27 +2076,12 @@
         <v>11</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="N10" s="41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>10</v>
@@ -2118,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
@@ -2127,9 +2102,9 @@
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>10</v>
@@ -2141,7 +2116,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
@@ -2150,7 +2125,7 @@
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
@@ -2166,8 +2141,8 @@
       <c r="F13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="43" t="s">
-        <v>52</v>
+      <c r="J13" s="42" t="s">
+        <v>51</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
@@ -2175,7 +2150,7 @@
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
     </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
@@ -2183,13 +2158,13 @@
         <v>28</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
@@ -2198,28 +2173,28 @@
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J15" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="54"/>
-      <c r="L15" s="55" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J15" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="M15" s="55" t="s">
+      <c r="M15" s="54" t="s">
         <v>1</v>
       </c>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
     </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="J16" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -2227,16 +2202,16 @@
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
     </row>
-    <row r="17" spans="2:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B17" s="81" t="s">
+    <row r="17" spans="2:15" ht="20" x14ac:dyDescent="0.3">
+      <c r="B17" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="83"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="87"/>
       <c r="J17" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
@@ -2244,7 +2219,7 @@
       <c r="N17" s="31"/>
       <c r="O17" s="31"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
@@ -2267,12 +2242,12 @@
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
     </row>
-    <row r="19" spans="2:15" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>11</v>
@@ -2283,30 +2258,30 @@
       <c r="F19" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="77" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" s="77"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
+      <c r="J19" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
       <c r="O19" s="31"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="45" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="46" t="s">
-        <v>40</v>
+      <c r="F20" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
@@ -2315,21 +2290,21 @@
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
     </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="47" t="s">
+    <row r="21" spans="2:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="49" t="s">
-        <v>40</v>
+      <c r="F21" s="48" t="s">
+        <v>39</v>
       </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
@@ -2338,7 +2313,7 @@
       <c r="N21" s="31"/>
       <c r="O21" s="31"/>
     </row>
-    <row r="22" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -2351,14 +2326,14 @@
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
     </row>
-    <row r="23" spans="2:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B23" s="78" t="s">
+    <row r="23" spans="2:15" ht="20" x14ac:dyDescent="0.3">
+      <c r="B23" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="80"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="84"/>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
@@ -2366,29 +2341,29 @@
       <c r="N23" s="31"/>
       <c r="O23" s="31"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="50" t="s">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="51" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>11</v>
@@ -2400,8 +2375,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
+    <row r="26" spans="2:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="52" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="35" t="s">
@@ -2414,20 +2389,20 @@
         <v>11</v>
       </c>
       <c r="F26" s="36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B29" s="81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:15" ht="20" x14ac:dyDescent="0.3">
+      <c r="B29" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="83"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="87"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>6</v>
       </c>
@@ -2444,9 +2419,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>10</v>
@@ -2461,7 +2436,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="17" t="s">
         <v>26</v>
       </c>
@@ -2475,11 +2450,11 @@
         <v>11</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G33" s="4"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
@@ -2487,26 +2462,26 @@
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="2"/>
       <c r="G34" s="4"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B35" s="81" t="s">
+    <row r="35" spans="1:15" ht="20" x14ac:dyDescent="0.3">
+      <c r="B35" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="83"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="87"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="6" t="s">
         <v>6</v>
@@ -2528,20 +2503,20 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B37" s="86" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="87" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="87" t="s">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B37" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="87" t="s">
+      <c r="E37" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="88" t="s">
+      <c r="F37" s="74" t="s">
         <v>24</v>
       </c>
       <c r="G37" s="4"/>
@@ -2549,28 +2524,28 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="90" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="90" t="s">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="90" t="s">
+      <c r="E38" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="91" t="s">
-        <v>40</v>
+      <c r="F38" s="77" t="s">
+        <v>39</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="20" t="s">
         <v>29</v>
       </c>
@@ -2578,13 +2553,13 @@
         <v>25</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="21" t="s">
         <v>1</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -2594,7 +2569,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2603,7 +2578,7 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -2613,7 +2588,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -2624,7 +2599,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2636,13 +2611,13 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F46" s="4"/>
     </row>
   </sheetData>
@@ -2667,10 +2642,10 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.25" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
@@ -2681,435 +2656,435 @@
     <col min="7" max="7" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="65"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="69" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+      <c r="A12" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="73" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="66" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="67" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="66" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="67" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B13" t="s">
         <v>103</v>
       </c>
-      <c r="E5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="67"/>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="69" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="66" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="70" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="64"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="62"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>